<commit_message>
new production, updated BOM about unused components
</commit_message>
<xml_diff>
--- a/resources/exixe12_bom.xlsx
+++ b/resources/exixe12_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\repos\exixe\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\Desktop\repos\exixe\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52AA257-D3E4-4528-BF33-3A0B66D98841}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFFBCBC-F862-457D-9C47-7C9D30B6E687}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exixe12" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +262,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -278,9 +284,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -667,7 +674,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1270,7 +1277,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>